<commit_message>
Updated for 2018 INFORMS Annual Meeting
</commit_message>
<xml_diff>
--- a/ESPNSportsAnalytics.xlsx
+++ b/ESPNSportsAnalytics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R Projects\espnsports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EF47087-1236-445F-A827-0552EB42C66E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FF5506-0D02-442B-B6C4-9F7577B0DAF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3855" xr2:uid="{7AEEE231-CE81-4326-8265-09CB82554642}"/>
   </bookViews>
@@ -966,7 +966,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1059,10 +1059,10 @@
         <v>2</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O2">
         <v>617594</v>
@@ -1153,10 +1153,10 @@
         <v>2</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>396698</v>
@@ -1200,10 +1200,10 @@
         <v>5</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O5">
         <v>2099451</v>
@@ -1247,10 +1247,10 @@
         <v>3</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <v>8622698</v>
@@ -1294,10 +1294,10 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>390724</v>
@@ -1576,10 +1576,10 @@
         <v>4</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O13">
         <v>3792621</v>
@@ -1905,10 +1905,10 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O20">
         <v>594833</v>
@@ -2140,10 +2140,10 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O25">
         <v>420003</v>
@@ -2457,10 +2457,10 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -2495,31 +2495,31 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
         <v>3</v>
       </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>2</v>
-      </c>
       <c r="M33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O33">
         <v>2099451</v>
@@ -2557,16 +2557,16 @@
         <v>0</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O34">
         <v>1580863</v>
@@ -2589,31 +2589,31 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35">
         <v>1</v>
       </c>
       <c r="J35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="L35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35">
         <v>1511946</v>
@@ -2636,25 +2636,25 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
       <c r="J36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -2680,10 +2680,10 @@
         <v>4</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K37">
         <v>1</v>
@@ -2704,10 +2704,10 @@
         <v>3</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O37">
         <v>617594</v>
@@ -2727,22 +2727,22 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I38">
         <v>1</v>
       </c>
       <c r="J38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -2751,10 +2751,10 @@
         <v>4</v>
       </c>
       <c r="M38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O38">
         <v>396698</v>
@@ -2780,16 +2780,16 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2824,19 +2824,19 @@
         <v>1</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
         <v>5</v>
-      </c>
-      <c r="I40">
-        <v>1</v>
-      </c>
-      <c r="J40">
-        <v>4</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -2845,10 +2845,10 @@
         <v>5</v>
       </c>
       <c r="M40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O40">
         <v>390724</v>
@@ -2868,16 +2868,16 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2915,22 +2915,22 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
         <v>3</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
       <c r="I42">
         <v>1</v>
       </c>
       <c r="J42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K42">
         <v>1</v>
@@ -2939,10 +2939,10 @@
         <v>1</v>
       </c>
       <c r="M42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42">
         <v>579999</v>
@@ -2965,19 +2965,19 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43">
         <v>1</v>
       </c>
       <c r="J43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K43">
         <v>1</v>
@@ -2986,10 +2986,10 @@
         <v>1</v>
       </c>
       <c r="M43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O43">
         <v>583776</v>
@@ -3009,22 +3009,22 @@
         <v>3</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -3056,16 +3056,16 @@
         <v>3</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -3080,10 +3080,10 @@
         <v>1</v>
       </c>
       <c r="M45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O45">
         <v>820445</v>
@@ -3103,34 +3103,34 @@
         <v>3</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46">
         <v>399457</v>
@@ -3150,22 +3150,22 @@
         <v>3</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -3174,10 +3174,10 @@
         <v>1</v>
       </c>
       <c r="M47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O47">
         <v>594833</v>
@@ -3347,13 +3347,13 @@
         <v>1</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I51">
         <v>1</v>
       </c>
       <c r="J51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -3362,10 +3362,10 @@
         <v>2</v>
       </c>
       <c r="M51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O51">
         <v>2731571</v>
@@ -3397,10 +3397,10 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -3409,10 +3409,10 @@
         <v>2</v>
       </c>
       <c r="M52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O52">
         <v>186440</v>
@@ -3435,25 +3435,25 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -3535,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="H55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55">
         <v>1</v>
@@ -3544,10 +3544,10 @@
         <v>1</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M55">
         <v>0</v>
@@ -3573,16 +3573,16 @@
         <v>2</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56">
         <v>1</v>
@@ -3597,10 +3597,10 @@
         <v>1</v>
       </c>
       <c r="M56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O56">
         <v>382578</v>
@@ -3620,16 +3620,16 @@
         <v>2</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -3638,16 +3638,16 @@
         <v>0</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O57">
         <v>343829</v>
@@ -3673,28 +3673,28 @@
         <v>2</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K58">
         <v>1</v>
       </c>
       <c r="L58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O58">
         <v>6131977</v>

</xml_diff>

<commit_message>
Updated for April 2019 Spaces RTA Presentation. Added 2018 NFL and corrected Raleigh spelling.
</commit_message>
<xml_diff>
--- a/ESPNSportsAnalytics.xlsx
+++ b/ESPNSportsAnalytics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R Projects\espnsports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FF5506-0D02-442B-B6C4-9F7577B0DAF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6054A02-72A4-4618-91C9-822D205C1AC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3855" xr2:uid="{7AEEE231-CE81-4326-8265-09CB82554642}"/>
+    <workbookView xWindow="12490" yWindow="1870" windowWidth="15360" windowHeight="7920" xr2:uid="{7AEEE231-CE81-4326-8265-09CB82554642}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -396,9 +396,6 @@
     <t>Hurricanes</t>
   </si>
   <si>
-    <t>Raliegh</t>
-  </si>
-  <si>
     <t>RedWings</t>
   </si>
   <si>
@@ -598,6 +595,9 @@
   </si>
   <si>
     <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
   </si>
 </sst>
 </file>
@@ -963,10 +963,10 @@
   <dimension ref="A1:O124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomRight" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -988,34 +988,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="O1" t="s">
         <v>99</v>
@@ -1828,7 +1828,7 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -3003,7 +3003,7 @@
         <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D44">
         <v>3</v>
@@ -3050,7 +3050,7 @@
         <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -3285,7 +3285,7 @@
         <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D50">
         <v>3</v>
@@ -3379,7 +3379,7 @@
         <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D52">
         <v>3</v>
@@ -4601,7 +4601,7 @@
         <v>121</v>
       </c>
       <c r="C78" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="D78">
         <v>3</v>
@@ -4645,7 +4645,7 @@
         <v>100</v>
       </c>
       <c r="B79" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C79" t="s">
         <v>61</v>
@@ -4692,7 +4692,7 @@
         <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C80" t="s">
         <v>52</v>
@@ -4739,10 +4739,10 @@
         <v>100</v>
       </c>
       <c r="B81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -4786,10 +4786,10 @@
         <v>100</v>
       </c>
       <c r="B82" t="s">
+        <v>124</v>
+      </c>
+      <c r="C82" t="s">
         <v>125</v>
-      </c>
-      <c r="C82" t="s">
-        <v>126</v>
       </c>
       <c r="D82">
         <v>3</v>
@@ -4833,10 +4833,10 @@
         <v>100</v>
       </c>
       <c r="B83" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" t="s">
         <v>127</v>
-      </c>
-      <c r="C83" t="s">
-        <v>128</v>
       </c>
       <c r="D83">
         <v>3</v>
@@ -4880,10 +4880,10 @@
         <v>100</v>
       </c>
       <c r="B84" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D84">
         <v>3</v>
@@ -4927,7 +4927,7 @@
         <v>100</v>
       </c>
       <c r="B85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C85" t="s">
         <v>58</v>
@@ -4974,10 +4974,10 @@
         <v>100</v>
       </c>
       <c r="B86" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" t="s">
         <v>131</v>
-      </c>
-      <c r="C86" t="s">
-        <v>132</v>
       </c>
       <c r="D86">
         <v>3</v>
@@ -5021,10 +5021,10 @@
         <v>100</v>
       </c>
       <c r="B87" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" t="s">
         <v>133</v>
-      </c>
-      <c r="C87" t="s">
-        <v>134</v>
       </c>
       <c r="D87">
         <v>3</v>
@@ -5068,10 +5068,10 @@
         <v>100</v>
       </c>
       <c r="B88" t="s">
+        <v>134</v>
+      </c>
+      <c r="C88" t="s">
         <v>135</v>
-      </c>
-      <c r="C88" t="s">
-        <v>136</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -5162,10 +5162,10 @@
         <v>100</v>
       </c>
       <c r="B90" t="s">
+        <v>136</v>
+      </c>
+      <c r="C90" t="s">
         <v>137</v>
-      </c>
-      <c r="C90" t="s">
-        <v>138</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -5209,7 +5209,7 @@
         <v>100</v>
       </c>
       <c r="B91" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C91" t="s">
         <v>90</v>
@@ -5253,10 +5253,10 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" t="s">
         <v>140</v>
-      </c>
-      <c r="B92" t="s">
-        <v>141</v>
       </c>
       <c r="C92" t="s">
         <v>47</v>
@@ -5300,10 +5300,10 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B93" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C93" t="s">
         <v>24</v>
@@ -5336,10 +5336,10 @@
         <v>0</v>
       </c>
       <c r="M93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O93">
         <v>620961</v>
@@ -5347,10 +5347,10 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
@@ -5394,10 +5394,10 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C95" t="s">
         <v>61</v>
@@ -5430,10 +5430,10 @@
         <v>0</v>
       </c>
       <c r="M95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N95">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O95">
         <v>1197816</v>
@@ -5441,13 +5441,13 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B96" t="s">
+        <v>144</v>
+      </c>
+      <c r="C96" t="s">
         <v>145</v>
-      </c>
-      <c r="C96" t="s">
-        <v>146</v>
       </c>
       <c r="D96">
         <v>4</v>
@@ -5488,10 +5488,10 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B97" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C97" t="s">
         <v>26</v>
@@ -5524,10 +5524,10 @@
         <v>1</v>
       </c>
       <c r="M97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N97">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O97">
         <v>2159159</v>
@@ -5535,10 +5535,10 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B98" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>
@@ -5571,10 +5571,10 @@
         <v>4</v>
       </c>
       <c r="M98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N98">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O98">
         <v>617594</v>
@@ -5582,10 +5582,10 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B99" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C99" t="s">
         <v>58</v>
@@ -5618,10 +5618,10 @@
         <v>5</v>
       </c>
       <c r="M99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N99">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O99">
         <v>1580863</v>
@@ -5629,10 +5629,10 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B100" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C100" t="s">
         <v>41</v>
@@ -5676,10 +5676,10 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B101" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C101" t="s">
         <v>104</v>
@@ -5723,10 +5723,10 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
@@ -5759,10 +5759,10 @@
         <v>0</v>
       </c>
       <c r="M102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O102">
         <v>2695598</v>
@@ -5770,13 +5770,13 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B103" t="s">
+        <v>152</v>
+      </c>
+      <c r="C103" t="s">
         <v>153</v>
-      </c>
-      <c r="C103" t="s">
-        <v>154</v>
       </c>
       <c r="D103">
         <v>3</v>
@@ -5817,10 +5817,10 @@
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B104" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C104" t="s">
         <v>56</v>
@@ -5864,10 +5864,10 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B105" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C105" t="s">
         <v>15</v>
@@ -5911,10 +5911,10 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B106" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C106" t="s">
         <v>43</v>
@@ -5947,10 +5947,10 @@
         <v>0</v>
       </c>
       <c r="M106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O106">
         <v>608660</v>
@@ -5958,10 +5958,10 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B107" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C107" t="s">
         <v>22</v>
@@ -6005,7 +6005,7 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B108" t="s">
         <v>18</v>
@@ -6052,13 +6052,13 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C109" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D109">
         <v>2</v>
@@ -6099,10 +6099,10 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C110" t="s">
         <v>49</v>
@@ -6146,10 +6146,10 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B111" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C111" t="s">
         <v>90</v>
@@ -6193,10 +6193,10 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B112" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C112" t="s">
         <v>52</v>
@@ -6240,10 +6240,10 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C113" t="s">
         <v>12</v>
@@ -6276,10 +6276,10 @@
         <v>0</v>
       </c>
       <c r="M113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O113">
         <v>2099451</v>
@@ -6287,14 +6287,14 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B114" t="s">
+        <v>162</v>
+      </c>
+      <c r="C114" t="s">
         <v>163</v>
       </c>
-      <c r="C114" t="s">
-        <v>164</v>
-      </c>
       <c r="D114">
         <v>2</v>
       </c>
@@ -6323,10 +6323,10 @@
         <v>0</v>
       </c>
       <c r="M114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N114">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O114">
         <v>820445</v>
@@ -6334,10 +6334,10 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B115" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C115" t="s">
         <v>54</v>
@@ -6381,10 +6381,10 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B116" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C116" t="s">
         <v>94</v>
@@ -6417,10 +6417,10 @@
         <v>2</v>
       </c>
       <c r="M116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N116">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O116">
         <v>343829</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B117" t="s">
         <v>40</v>
@@ -6475,10 +6475,10 @@
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B118" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C118" t="s">
         <v>17</v>
@@ -6522,10 +6522,10 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B119" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C119" t="s">
         <v>28</v>
@@ -6558,10 +6558,10 @@
         <v>1</v>
       </c>
       <c r="M119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N119">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O119">
         <v>3792621</v>
@@ -6569,7 +6569,7 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B120" t="s">
         <v>116</v>
@@ -6616,10 +6616,10 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B121" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C121" t="s">
         <v>28</v>
@@ -6652,10 +6652,10 @@
         <v>0</v>
       </c>
       <c r="M121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N121">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O121">
         <v>3792621</v>
@@ -6663,13 +6663,13 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B122" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C122" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -6710,10 +6710,10 @@
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B123" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C123" t="s">
         <v>35</v>
@@ -6760,10 +6760,10 @@
         <v>100</v>
       </c>
       <c r="B124" t="s">
+        <v>182</v>
+      </c>
+      <c r="C124" t="s">
         <v>183</v>
-      </c>
-      <c r="C124" t="s">
-        <v>184</v>
       </c>
       <c r="D124">
         <v>5</v>

</xml_diff>